<commit_message>
Todavia con error en Fink
</commit_message>
<xml_diff>
--- a/codigo/repaso_matricial/general_2D/fink.xlsx
+++ b/codigo/repaso_matricial/general_2D/fink.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALTA ORGANIZAR</t>
   </si>
   <si>
     <t xml:space="preserve">EF</t>
@@ -455,12 +452,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -497,7 +500,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -512,6 +515,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -561,9 +568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -573,7 +580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -606,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -618,7 +625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -656,9 +663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>686520</xdr:colOff>
+      <xdr:colOff>685080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -668,7 +675,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10050840" cy="9517320"/>
+          <a:ext cx="10094040" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -701,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>686520</xdr:colOff>
+      <xdr:colOff>685080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -713,7 +720,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10050840" cy="9517320"/>
+          <a:ext cx="10094040" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,9 +758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -763,7 +770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -796,9 +803,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -808,7 +815,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -841,9 +848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -853,7 +860,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,9 +893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -898,7 +905,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -936,9 +943,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -948,7 +955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -981,9 +988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>286560</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -993,7 +1000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10089360" cy="9517320"/>
+          <a:ext cx="10141200" cy="9515880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1027,11 +1034,11 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1136,9 +1143,6 @@
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>3</v>
-      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
@@ -1247,26 +1251,26 @@
       <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,7 +1341,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1355,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1485,10 +1489,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -1498,13 +1502,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,18 +1546,57 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1580,23 +1623,23 @@
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1604,16 +1647,16 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="n">
+      <c r="B2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1621,16 +1664,16 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="n">
+      <c r="B3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1638,16 +1681,16 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4" t="n">
+      <c r="B4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1655,16 +1698,16 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="n">
+      <c r="B5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1672,16 +1715,16 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="n">
+      <c r="B6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1689,16 +1732,16 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="n">
+      <c r="B7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1706,16 +1749,16 @@
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="n">
+      <c r="B8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1723,16 +1766,16 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="n">
+      <c r="B9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1740,16 +1783,16 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="n">
+      <c r="B10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1757,16 +1800,16 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="n">
+      <c r="B11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1774,60 +1817,60 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4" t="n">
+      <c r="B12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1850,20 +1893,20 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,7 +1949,7 @@
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <f aca="false">-10*COS(ang1)</f>
         <v>-5.54700196225229</v>
       </c>
@@ -1918,7 +1961,7 @@
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <f aca="false">-10*SIN(ang1)</f>
         <v>-8.32050294337844</v>
       </c>
@@ -1930,7 +1973,7 @@
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <f aca="false">-20*COS(ang1)</f>
         <v>-11.0940039245046</v>
       </c>
@@ -1942,7 +1985,7 @@
       <c r="B8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <f aca="false">-20*SIN(ang1)</f>
         <v>-16.6410058867569</v>
       </c>
@@ -1954,7 +1997,7 @@
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="6" t="n">
         <f aca="false">-10*COS(ang1)</f>
         <v>-5.54700196225229</v>
       </c>
@@ -1966,7 +2009,7 @@
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="6" t="n">
         <f aca="false">-10*SIN(ang1)</f>
         <v>-8.32050294337844</v>
       </c>
@@ -1991,42 +2034,42 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>200000000</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">PI()*0.04^2</f>
         <v>0.00502654824574367</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <f aca="false">PI()*0.04^4/4</f>
         <v>2.01061929829747E-006</v>
       </c>
@@ -2038,7 +2081,7 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>200000000</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -2073,65 +2116,65 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="B5" s="0" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2152,72 +2195,72 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="0" t="n">
         <f aca="false">ATAN2(3,4.5)</f>
         <v>0.982793723247329</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="9" t="n">
+        <v>34</v>
+      </c>
+      <c r="D1" s="10" t="n">
         <f aca="false">DEGREES(B1)</f>
         <v>56.3099324740202</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando ejemplo de estructura Fink
</commit_message>
<xml_diff>
--- a/codigo/repaso_matricial/general_2D/fink.xlsx
+++ b/codigo/repaso_matricial/general_2D/fink.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -568,9 +568,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -580,7 +580,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -613,9 +613,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -625,7 +625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -663,9 +663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>685080</xdr:colOff>
+      <xdr:colOff>684360</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -675,7 +675,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10094040" cy="9515880"/>
+          <a:ext cx="10118520" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>685080</xdr:colOff>
+      <xdr:colOff>684360</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -720,7 +720,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10094040" cy="9515880"/>
+          <a:ext cx="10118520" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -758,9 +758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -770,7 +770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,9 +803,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -815,7 +815,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -848,9 +848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -860,7 +860,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -893,9 +893,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -905,7 +905,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -943,9 +943,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -955,7 +955,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -988,9 +988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
+      <xdr:colOff>284400</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1000,7 +1000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="10141200" cy="9515880"/>
+          <a:ext cx="10170720" cy="9515160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1038,7 +1038,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1251,7 +1251,7 @@
       <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.92"/>
   </cols>
@@ -1488,11 +1488,11 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -1516,8 +1516,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">X</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -1528,17 +1527,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">Y</f>
-        <v>2</v>
-      </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>-30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1621,7 @@
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1896,7 +1894,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2034,11 +2032,11 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -2119,7 +2117,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -2199,7 +2197,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>